<commit_message>
Algorythm figured out, restarting from testing perspective, building test methods first. Working in Unity because of incompatability between .NETCore & NUnit.Framework that I could not resolve quickly enough for the deadline. Once project is in unity, will abandon updating console executable and move it to an archived state.
</commit_message>
<xml_diff>
--- a/RomanNumeralParser/Tests/TestInputData.xlsx
+++ b/RomanNumeralParser/Tests/TestInputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopher/Documents/gitroot/InterviewProjects/RomanNumeralParser/RomanNumeralParser/Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFE7A15-8E81-ED49-8E45-22D521EDDCD7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECDB5AA-D763-1C4A-8F71-8134AB6A9E3A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="10260" windowWidth="22840" windowHeight="17440" activeTab="2" xr2:uid="{91AFFFCB-508E-A543-B8CF-427361C66550}"/>
   </bookViews>
@@ -11484,7 +11484,7 @@
   <dimension ref="A1:BS10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="AA12" sqref="AA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>